<commit_message>
removed notes and textual edit to mapping excel
</commit_message>
<xml_diff>
--- a/Profiles-Staging/NursingIntervention - STU3.xlsx
+++ b/Profiles-Staging/NursingIntervention - STU3.xlsx
@@ -5,17 +5,17 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MirjamB\Dropbox\Documenten\Zakelijk\Nictiz\4ZIBs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git\nicitz-stu3-zibs2017\Profiles-Staging\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8196" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="NursingIntervention 2017" sheetId="1" r:id="rId1"/>
     <sheet name="Valuesets 2017" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="0" iterate="1" iterateDelta="1E-4"/>
+  <calcPr calcId="0" iterate="1"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="ExcelA1"/>
@@ -557,79 +557,79 @@
   </cellStyleXfs>
   <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -983,13 +983,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:R19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G9" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L18" sqref="L18"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="8.5546875" customWidth="1"/>
+    <col min="1" max="1" width="8.5703125" customWidth="1"/>
     <col min="2" max="6" width="2" customWidth="1"/>
     <col min="7" max="7" width="15" customWidth="1"/>
     <col min="8" max="8" width="25" customWidth="1"/>
@@ -997,619 +997,619 @@
     <col min="11" max="11" width="12" customWidth="1"/>
     <col min="12" max="12" width="15" customWidth="1"/>
     <col min="13" max="13" width="75" customWidth="1"/>
-    <col min="14" max="14" width="20" customWidth="1"/>
-    <col min="15" max="15" width="30" customWidth="1"/>
-    <col min="16" max="16" width="21.44140625" customWidth="1"/>
-    <col min="17" max="17" width="20.44140625" customWidth="1"/>
-    <col min="18" max="1025" width="8.5546875" customWidth="1"/>
+    <col min="14" max="14" width="20" hidden="1" customWidth="1"/>
+    <col min="15" max="15" width="30" hidden="1" customWidth="1"/>
+    <col min="16" max="16" width="32.42578125" customWidth="1"/>
+    <col min="17" max="17" width="31.140625" customWidth="1"/>
+    <col min="18" max="1025" width="8.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:18" ht="27.6" x14ac:dyDescent="0.3">
-      <c r="B2" s="4" t="s">
+    <row r="2" spans="2:18" x14ac:dyDescent="0.2">
+      <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="5"/>
-      <c r="D2" s="5"/>
-      <c r="E2" s="5"/>
-      <c r="F2" s="5"/>
-      <c r="G2" s="6"/>
-      <c r="H2" s="7" t="s">
+      <c r="C2" s="2"/>
+      <c r="D2" s="2"/>
+      <c r="E2" s="2"/>
+      <c r="F2" s="2"/>
+      <c r="G2" s="3"/>
+      <c r="H2" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="I2" s="7" t="s">
+      <c r="I2" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="J2" s="7" t="s">
+      <c r="J2" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="K2" s="7" t="s">
+      <c r="K2" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="L2" s="7" t="s">
+      <c r="L2" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="M2" s="7" t="s">
+      <c r="M2" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="N2" s="7" t="s">
+      <c r="N2" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="O2" s="7" t="s">
+      <c r="O2" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="P2" s="7" t="s">
+      <c r="P2" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="Q2" s="7" t="s">
+      <c r="Q2" s="4" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="2:18" ht="27.6" x14ac:dyDescent="0.3">
-      <c r="B3" s="8" t="s">
+    <row r="3" spans="2:18" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="B3" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="C3" s="9"/>
-      <c r="D3" s="9"/>
-      <c r="E3" s="9"/>
-      <c r="F3" s="9"/>
-      <c r="G3" s="10"/>
-      <c r="H3" s="11" t="s">
+      <c r="C3" s="6"/>
+      <c r="D3" s="6"/>
+      <c r="E3" s="6"/>
+      <c r="F3" s="6"/>
+      <c r="G3" s="7"/>
+      <c r="H3" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="I3" s="11"/>
-      <c r="J3" s="11"/>
-      <c r="K3" s="11" t="s">
+      <c r="I3" s="8"/>
+      <c r="J3" s="8"/>
+      <c r="K3" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="L3" s="11" t="s">
+      <c r="L3" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="M3" s="11" t="s">
+      <c r="M3" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="N3" s="11"/>
-      <c r="O3" s="11"/>
-      <c r="P3" s="11" t="s">
+      <c r="N3" s="8"/>
+      <c r="O3" s="8"/>
+      <c r="P3" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="Q3" s="12"/>
-    </row>
-    <row r="4" spans="2:18" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="13"/>
-      <c r="C4" s="14" t="s">
+      <c r="Q3" s="9"/>
+    </row>
+    <row r="4" spans="2:18" x14ac:dyDescent="0.2">
+      <c r="B4" s="10"/>
+      <c r="C4" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="D4" s="14"/>
-      <c r="E4" s="14"/>
-      <c r="F4" s="14"/>
-      <c r="G4" s="15"/>
-      <c r="H4" s="3" t="s">
+      <c r="D4" s="11"/>
+      <c r="E4" s="11"/>
+      <c r="F4" s="11"/>
+      <c r="G4" s="12"/>
+      <c r="H4" s="23" t="s">
         <v>18</v>
       </c>
-      <c r="I4" s="3" t="s">
+      <c r="I4" s="23" t="s">
         <v>19</v>
       </c>
-      <c r="J4" s="3" t="s">
+      <c r="J4" s="23" t="s">
         <v>20</v>
       </c>
-      <c r="K4" s="3" t="s">
+      <c r="K4" s="23" t="s">
         <v>21</v>
       </c>
-      <c r="L4" s="3" t="s">
+      <c r="L4" s="23" t="s">
         <v>22</v>
       </c>
-      <c r="M4" s="3" t="s">
+      <c r="M4" s="23" t="s">
         <v>23</v>
       </c>
-      <c r="N4" s="3"/>
-      <c r="O4" s="17" t="s">
+      <c r="N4" s="23"/>
+      <c r="O4" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="P4" s="3" t="s">
+      <c r="P4" s="23" t="s">
         <v>25</v>
       </c>
-      <c r="Q4" s="2" t="s">
+      <c r="Q4" s="24" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="5" spans="2:18" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="13"/>
-      <c r="C5" s="14"/>
-      <c r="D5" s="14"/>
-      <c r="E5" s="14"/>
-      <c r="F5" s="14"/>
-      <c r="G5" s="15"/>
-      <c r="H5" s="3"/>
-      <c r="I5" s="3"/>
-      <c r="J5" s="3"/>
-      <c r="K5" s="3"/>
-      <c r="L5" s="3"/>
-      <c r="M5" s="3"/>
-      <c r="N5" s="3"/>
-      <c r="O5" s="17" t="s">
+    <row r="5" spans="2:18" x14ac:dyDescent="0.2">
+      <c r="B5" s="10"/>
+      <c r="C5" s="11"/>
+      <c r="D5" s="11"/>
+      <c r="E5" s="11"/>
+      <c r="F5" s="11"/>
+      <c r="G5" s="12"/>
+      <c r="H5" s="23"/>
+      <c r="I5" s="23"/>
+      <c r="J5" s="23"/>
+      <c r="K5" s="23"/>
+      <c r="L5" s="23"/>
+      <c r="M5" s="23"/>
+      <c r="N5" s="23"/>
+      <c r="O5" s="14" t="s">
         <v>27</v>
       </c>
-      <c r="P5" s="3"/>
-      <c r="Q5" s="2"/>
-    </row>
-    <row r="6" spans="2:18" ht="41.4" x14ac:dyDescent="0.3">
-      <c r="B6" s="13"/>
-      <c r="C6" s="14" t="s">
+      <c r="P5" s="23"/>
+      <c r="Q5" s="24"/>
+    </row>
+    <row r="6" spans="2:18" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="B6" s="10"/>
+      <c r="C6" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="D6" s="14"/>
-      <c r="E6" s="14"/>
-      <c r="F6" s="14"/>
-      <c r="G6" s="15"/>
-      <c r="H6" s="16" t="s">
+      <c r="D6" s="11"/>
+      <c r="E6" s="11"/>
+      <c r="F6" s="11"/>
+      <c r="G6" s="12"/>
+      <c r="H6" s="13" t="s">
         <v>29</v>
       </c>
-      <c r="I6" s="16"/>
-      <c r="J6" s="16" t="s">
+      <c r="I6" s="13"/>
+      <c r="J6" s="13" t="s">
         <v>30</v>
       </c>
-      <c r="K6" s="16" t="s">
+      <c r="K6" s="13" t="s">
         <v>31</v>
       </c>
-      <c r="L6" s="16" t="s">
+      <c r="L6" s="13" t="s">
         <v>32</v>
       </c>
-      <c r="M6" s="16" t="s">
+      <c r="M6" s="13" t="s">
         <v>33</v>
       </c>
-      <c r="N6" s="16"/>
-      <c r="O6" s="17" t="s">
+      <c r="N6" s="13"/>
+      <c r="O6" s="14" t="s">
         <v>34</v>
       </c>
-      <c r="P6" s="16" t="s">
+      <c r="P6" s="13" t="s">
         <v>35</v>
       </c>
-      <c r="Q6" s="12"/>
-    </row>
-    <row r="7" spans="2:18" ht="41.4" x14ac:dyDescent="0.3">
-      <c r="B7" s="13"/>
-      <c r="C7" s="14" t="s">
+      <c r="Q6" s="9"/>
+    </row>
+    <row r="7" spans="2:18" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="B7" s="10"/>
+      <c r="C7" s="11" t="s">
         <v>36</v>
       </c>
-      <c r="D7" s="14"/>
-      <c r="E7" s="14"/>
-      <c r="F7" s="14"/>
-      <c r="G7" s="15"/>
-      <c r="H7" s="16" t="s">
+      <c r="D7" s="11"/>
+      <c r="E7" s="11"/>
+      <c r="F7" s="11"/>
+      <c r="G7" s="12"/>
+      <c r="H7" s="13" t="s">
         <v>37</v>
       </c>
-      <c r="I7" s="16"/>
-      <c r="J7" s="16" t="s">
+      <c r="I7" s="13"/>
+      <c r="J7" s="13" t="s">
         <v>30</v>
       </c>
-      <c r="K7" s="16" t="s">
+      <c r="K7" s="13" t="s">
         <v>31</v>
       </c>
-      <c r="L7" s="16" t="s">
+      <c r="L7" s="13" t="s">
         <v>38</v>
       </c>
-      <c r="M7" s="16" t="s">
+      <c r="M7" s="13" t="s">
         <v>39</v>
       </c>
-      <c r="N7" s="16"/>
-      <c r="O7" s="17" t="s">
+      <c r="N7" s="13"/>
+      <c r="O7" s="14" t="s">
         <v>40</v>
       </c>
-      <c r="P7" s="16" t="s">
+      <c r="P7" s="13" t="s">
         <v>41</v>
       </c>
-      <c r="Q7" s="12"/>
-    </row>
-    <row r="8" spans="2:18" ht="41.4" x14ac:dyDescent="0.3">
-      <c r="B8" s="13"/>
-      <c r="C8" s="14" t="s">
+      <c r="Q7" s="9"/>
+    </row>
+    <row r="8" spans="2:18" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="B8" s="10"/>
+      <c r="C8" s="11" t="s">
         <v>42</v>
       </c>
-      <c r="D8" s="14"/>
-      <c r="E8" s="14"/>
-      <c r="F8" s="14"/>
-      <c r="G8" s="15"/>
-      <c r="H8" s="16" t="s">
+      <c r="D8" s="11"/>
+      <c r="E8" s="11"/>
+      <c r="F8" s="11"/>
+      <c r="G8" s="12"/>
+      <c r="H8" s="13" t="s">
         <v>43</v>
       </c>
-      <c r="I8" s="16" t="s">
+      <c r="I8" s="13" t="s">
         <v>44</v>
       </c>
-      <c r="J8" s="16" t="s">
+      <c r="J8" s="13" t="s">
         <v>30</v>
       </c>
-      <c r="K8" s="16" t="s">
+      <c r="K8" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="L8" s="16" t="s">
+      <c r="L8" s="13" t="s">
         <v>45</v>
       </c>
-      <c r="M8" s="16" t="s">
+      <c r="M8" s="13" t="s">
         <v>46</v>
       </c>
-      <c r="N8" s="16"/>
-      <c r="P8" s="16" t="s">
+      <c r="N8" s="13"/>
+      <c r="P8" s="13" t="s">
         <v>119</v>
       </c>
-      <c r="Q8" s="12"/>
-    </row>
-    <row r="9" spans="2:18" ht="34.799999999999997" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="13"/>
-      <c r="C9" s="14" t="s">
+      <c r="Q8" s="9"/>
+    </row>
+    <row r="9" spans="2:18" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="B9" s="10"/>
+      <c r="C9" s="11" t="s">
         <v>47</v>
       </c>
-      <c r="D9" s="14"/>
-      <c r="E9" s="14"/>
-      <c r="F9" s="14"/>
-      <c r="G9" s="15"/>
-      <c r="H9" s="16" t="s">
+      <c r="D9" s="11"/>
+      <c r="E9" s="11"/>
+      <c r="F9" s="11"/>
+      <c r="G9" s="12"/>
+      <c r="H9" s="13" t="s">
         <v>48</v>
       </c>
-      <c r="I9" s="16" t="s">
+      <c r="I9" s="13" t="s">
         <v>44</v>
       </c>
-      <c r="J9" s="16" t="s">
+      <c r="J9" s="13" t="s">
         <v>30</v>
       </c>
-      <c r="K9" s="16" t="s">
+      <c r="K9" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="L9" s="16" t="s">
+      <c r="L9" s="13" t="s">
         <v>49</v>
       </c>
-      <c r="M9" s="16" t="s">
+      <c r="M9" s="13" t="s">
         <v>50</v>
       </c>
-      <c r="N9" s="16"/>
-      <c r="O9" s="16"/>
-      <c r="P9" s="16" t="s">
+      <c r="N9" s="13"/>
+      <c r="O9" s="13"/>
+      <c r="P9" s="13" t="s">
         <v>120</v>
       </c>
-      <c r="Q9" s="12"/>
-      <c r="R9" s="18"/>
-    </row>
-    <row r="10" spans="2:18" ht="35.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="13"/>
-      <c r="C10" s="14" t="s">
+      <c r="Q9" s="9"/>
+      <c r="R9" s="15"/>
+    </row>
+    <row r="10" spans="2:18" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="B10" s="10"/>
+      <c r="C10" s="11" t="s">
         <v>51</v>
       </c>
-      <c r="D10" s="14"/>
-      <c r="E10" s="14"/>
-      <c r="F10" s="14"/>
-      <c r="G10" s="15"/>
-      <c r="H10" s="16" t="s">
+      <c r="D10" s="11"/>
+      <c r="E10" s="11"/>
+      <c r="F10" s="11"/>
+      <c r="G10" s="12"/>
+      <c r="H10" s="13" t="s">
         <v>52</v>
       </c>
-      <c r="I10" s="16" t="s">
+      <c r="I10" s="13" t="s">
         <v>53</v>
       </c>
-      <c r="J10" s="16" t="s">
+      <c r="J10" s="13" t="s">
         <v>30</v>
       </c>
-      <c r="K10" s="16" t="s">
+      <c r="K10" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="L10" s="16" t="s">
+      <c r="L10" s="13" t="s">
         <v>54</v>
       </c>
-      <c r="M10" s="16" t="s">
+      <c r="M10" s="13" t="s">
         <v>55</v>
       </c>
-      <c r="N10" s="16"/>
-      <c r="O10" s="17"/>
-      <c r="P10" s="16" t="s">
+      <c r="N10" s="13"/>
+      <c r="O10" s="14"/>
+      <c r="P10" s="13" t="s">
         <v>56</v>
       </c>
-      <c r="Q10" s="12"/>
-    </row>
-    <row r="11" spans="2:18" ht="35.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="13"/>
-      <c r="C11" s="14" t="s">
+      <c r="Q10" s="9"/>
+    </row>
+    <row r="11" spans="2:18" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="B11" s="10"/>
+      <c r="C11" s="11" t="s">
         <v>57</v>
       </c>
-      <c r="D11" s="14"/>
-      <c r="E11" s="14"/>
-      <c r="F11" s="14"/>
-      <c r="G11" s="15"/>
-      <c r="H11" s="16" t="s">
+      <c r="D11" s="11"/>
+      <c r="E11" s="11"/>
+      <c r="F11" s="11"/>
+      <c r="G11" s="12"/>
+      <c r="H11" s="13" t="s">
         <v>58</v>
       </c>
-      <c r="I11" s="16" t="s">
+      <c r="I11" s="13" t="s">
         <v>53</v>
       </c>
-      <c r="J11" s="16" t="s">
+      <c r="J11" s="13" t="s">
         <v>30</v>
       </c>
-      <c r="K11" s="16" t="s">
+      <c r="K11" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="L11" s="16" t="s">
+      <c r="L11" s="13" t="s">
         <v>59</v>
       </c>
-      <c r="M11" s="16" t="s">
+      <c r="M11" s="13" t="s">
         <v>60</v>
       </c>
-      <c r="N11" s="16"/>
-      <c r="O11" s="17"/>
-      <c r="P11" s="16" t="s">
+      <c r="N11" s="13"/>
+      <c r="O11" s="14"/>
+      <c r="P11" s="13" t="s">
         <v>61</v>
       </c>
-      <c r="Q11" s="12"/>
-    </row>
-    <row r="12" spans="2:18" ht="34.799999999999997" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="13"/>
-      <c r="C12" s="14" t="s">
+      <c r="Q11" s="9"/>
+    </row>
+    <row r="12" spans="2:18" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="B12" s="10"/>
+      <c r="C12" s="11" t="s">
         <v>62</v>
       </c>
-      <c r="D12" s="14"/>
-      <c r="E12" s="14"/>
-      <c r="F12" s="14"/>
-      <c r="G12" s="15"/>
-      <c r="H12" s="16" t="s">
+      <c r="D12" s="11"/>
+      <c r="E12" s="11"/>
+      <c r="F12" s="11"/>
+      <c r="G12" s="12"/>
+      <c r="H12" s="13" t="s">
         <v>63</v>
       </c>
-      <c r="I12" s="16"/>
-      <c r="J12" s="16" t="s">
+      <c r="I12" s="13"/>
+      <c r="J12" s="13" t="s">
         <v>64</v>
       </c>
-      <c r="K12" s="16" t="s">
+      <c r="K12" s="13" t="s">
         <v>31</v>
       </c>
-      <c r="L12" s="16" t="s">
+      <c r="L12" s="13" t="s">
         <v>65</v>
       </c>
-      <c r="M12" s="16" t="s">
+      <c r="M12" s="13" t="s">
         <v>66</v>
       </c>
-      <c r="N12" s="16"/>
-      <c r="O12" s="17" t="s">
+      <c r="N12" s="13"/>
+      <c r="O12" s="14" t="s">
         <v>67</v>
       </c>
-      <c r="P12" s="16" t="s">
+      <c r="P12" s="13" t="s">
         <v>68</v>
       </c>
-      <c r="Q12" s="12"/>
-      <c r="R12" s="18"/>
-    </row>
-    <row r="13" spans="2:18" ht="34.799999999999997" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B13" s="13"/>
-      <c r="C13" s="14" t="s">
+      <c r="Q12" s="9"/>
+      <c r="R12" s="15"/>
+    </row>
+    <row r="13" spans="2:18" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="B13" s="10"/>
+      <c r="C13" s="11" t="s">
         <v>69</v>
       </c>
-      <c r="D13" s="14"/>
-      <c r="E13" s="14"/>
-      <c r="F13" s="14"/>
-      <c r="G13" s="15"/>
-      <c r="H13" s="16" t="s">
+      <c r="D13" s="11"/>
+      <c r="E13" s="11"/>
+      <c r="F13" s="11"/>
+      <c r="G13" s="12"/>
+      <c r="H13" s="13" t="s">
         <v>70</v>
       </c>
-      <c r="I13" s="16" t="s">
+      <c r="I13" s="13" t="s">
         <v>71</v>
       </c>
-      <c r="J13" s="16" t="s">
+      <c r="J13" s="13" t="s">
         <v>30</v>
       </c>
-      <c r="K13" s="16" t="s">
+      <c r="K13" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="L13" s="16" t="s">
+      <c r="L13" s="13" t="s">
         <v>72</v>
       </c>
-      <c r="M13" s="16" t="s">
+      <c r="M13" s="13" t="s">
         <v>73</v>
       </c>
-      <c r="N13" s="16"/>
-      <c r="O13" s="16"/>
-      <c r="P13" s="16" t="s">
+      <c r="N13" s="13"/>
+      <c r="O13" s="13"/>
+      <c r="P13" s="13" t="s">
         <v>121</v>
       </c>
-      <c r="Q13" s="12"/>
-      <c r="R13" s="18"/>
-    </row>
-    <row r="14" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B14" s="19"/>
-      <c r="C14" s="20" t="s">
+      <c r="Q13" s="9"/>
+      <c r="R13" s="15"/>
+    </row>
+    <row r="14" spans="2:18" x14ac:dyDescent="0.2">
+      <c r="B14" s="16"/>
+      <c r="C14" s="17" t="s">
         <v>74</v>
       </c>
-      <c r="D14" s="20"/>
-      <c r="E14" s="20"/>
-      <c r="F14" s="20"/>
-      <c r="G14" s="21"/>
-      <c r="H14" s="22" t="s">
+      <c r="D14" s="17"/>
+      <c r="E14" s="17"/>
+      <c r="F14" s="17"/>
+      <c r="G14" s="18"/>
+      <c r="H14" s="19" t="s">
         <v>75</v>
       </c>
-      <c r="I14" s="22"/>
-      <c r="J14" s="22" t="s">
+      <c r="I14" s="19"/>
+      <c r="J14" s="19" t="s">
         <v>30</v>
       </c>
-      <c r="K14" s="22" t="s">
+      <c r="K14" s="19" t="s">
         <v>76</v>
       </c>
-      <c r="L14" s="22" t="s">
+      <c r="L14" s="19" t="s">
         <v>77</v>
       </c>
-      <c r="M14" s="22" t="s">
+      <c r="M14" s="19" t="s">
         <v>78</v>
       </c>
-      <c r="N14" s="22"/>
-      <c r="O14" s="22"/>
-      <c r="P14" s="23" t="s">
+      <c r="N14" s="19"/>
+      <c r="O14" s="19"/>
+      <c r="P14" s="20" t="s">
         <v>79</v>
       </c>
-      <c r="Q14" s="12"/>
-    </row>
-    <row r="15" spans="2:18" ht="41.4" x14ac:dyDescent="0.3">
-      <c r="B15" s="13"/>
-      <c r="C15" s="24"/>
-      <c r="D15" s="24" t="s">
+      <c r="Q14" s="9"/>
+    </row>
+    <row r="15" spans="2:18" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="B15" s="10"/>
+      <c r="C15" s="21"/>
+      <c r="D15" s="21" t="s">
         <v>80</v>
       </c>
-      <c r="E15" s="24"/>
-      <c r="F15" s="24"/>
-      <c r="G15" s="15"/>
-      <c r="H15" s="16" t="s">
+      <c r="E15" s="21"/>
+      <c r="F15" s="21"/>
+      <c r="G15" s="12"/>
+      <c r="H15" s="13" t="s">
         <v>81</v>
       </c>
-      <c r="I15" s="16"/>
-      <c r="J15" s="16" t="s">
+      <c r="I15" s="13"/>
+      <c r="J15" s="13" t="s">
         <v>30</v>
       </c>
-      <c r="K15" s="16" t="s">
+      <c r="K15" s="13" t="s">
         <v>82</v>
       </c>
-      <c r="L15" s="16" t="s">
+      <c r="L15" s="13" t="s">
         <v>83</v>
       </c>
-      <c r="M15" s="16" t="s">
+      <c r="M15" s="13" t="s">
         <v>84</v>
       </c>
-      <c r="N15" s="16"/>
-      <c r="O15" s="17" t="s">
+      <c r="N15" s="13"/>
+      <c r="O15" s="14" t="s">
         <v>85</v>
       </c>
-      <c r="P15" s="16" t="s">
+      <c r="P15" s="13" t="s">
         <v>86</v>
       </c>
-      <c r="Q15" s="12"/>
-    </row>
-    <row r="16" spans="2:18" ht="41.4" x14ac:dyDescent="0.3">
-      <c r="B16" s="13"/>
-      <c r="C16" s="24"/>
-      <c r="D16" s="24" t="s">
+      <c r="Q15" s="9"/>
+    </row>
+    <row r="16" spans="2:18" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="B16" s="10"/>
+      <c r="C16" s="21"/>
+      <c r="D16" s="21" t="s">
         <v>87</v>
       </c>
-      <c r="E16" s="24"/>
-      <c r="F16" s="24"/>
-      <c r="G16" s="15"/>
-      <c r="H16" s="16" t="s">
+      <c r="E16" s="21"/>
+      <c r="F16" s="21"/>
+      <c r="G16" s="12"/>
+      <c r="H16" s="13" t="s">
         <v>88</v>
       </c>
-      <c r="I16" s="16"/>
-      <c r="J16" s="16" t="s">
+      <c r="I16" s="13"/>
+      <c r="J16" s="13" t="s">
         <v>30</v>
       </c>
-      <c r="K16" s="16" t="s">
+      <c r="K16" s="13" t="s">
         <v>82</v>
       </c>
-      <c r="L16" s="16" t="s">
+      <c r="L16" s="13" t="s">
         <v>89</v>
       </c>
-      <c r="M16" s="16" t="s">
+      <c r="M16" s="13" t="s">
         <v>90</v>
       </c>
-      <c r="N16" s="16"/>
-      <c r="O16" s="17" t="s">
+      <c r="N16" s="13"/>
+      <c r="O16" s="14" t="s">
         <v>91</v>
       </c>
-      <c r="P16" s="16" t="s">
+      <c r="P16" s="13" t="s">
         <v>86</v>
       </c>
-      <c r="Q16" s="12"/>
-      <c r="R16" s="18"/>
-    </row>
-    <row r="17" spans="2:17" ht="41.4" x14ac:dyDescent="0.3">
-      <c r="B17" s="13"/>
-      <c r="C17" s="24"/>
-      <c r="D17" s="24" t="s">
+      <c r="Q16" s="9"/>
+      <c r="R16" s="15"/>
+    </row>
+    <row r="17" spans="2:17" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="B17" s="10"/>
+      <c r="C17" s="21"/>
+      <c r="D17" s="21" t="s">
         <v>92</v>
       </c>
-      <c r="E17" s="24"/>
-      <c r="F17" s="24"/>
-      <c r="G17" s="15"/>
-      <c r="H17" s="16" t="s">
+      <c r="E17" s="21"/>
+      <c r="F17" s="21"/>
+      <c r="G17" s="12"/>
+      <c r="H17" s="13" t="s">
         <v>93</v>
       </c>
-      <c r="I17" s="16"/>
-      <c r="J17" s="16" t="s">
+      <c r="I17" s="13"/>
+      <c r="J17" s="13" t="s">
         <v>30</v>
       </c>
-      <c r="K17" s="16" t="s">
+      <c r="K17" s="13" t="s">
         <v>82</v>
       </c>
-      <c r="L17" s="16" t="s">
+      <c r="L17" s="13" t="s">
         <v>94</v>
       </c>
-      <c r="M17" s="16" t="s">
+      <c r="M17" s="13" t="s">
         <v>95</v>
       </c>
-      <c r="N17" s="16"/>
-      <c r="O17" s="17" t="s">
+      <c r="N17" s="13"/>
+      <c r="O17" s="14" t="s">
         <v>96</v>
       </c>
-      <c r="P17" s="16" t="s">
+      <c r="P17" s="13" t="s">
         <v>86</v>
       </c>
-      <c r="Q17" s="12"/>
-    </row>
-    <row r="18" spans="2:17" ht="41.4" x14ac:dyDescent="0.3">
-      <c r="B18" s="13"/>
-      <c r="C18" s="24" t="s">
+      <c r="Q17" s="9"/>
+    </row>
+    <row r="18" spans="2:17" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="B18" s="10"/>
+      <c r="C18" s="21" t="s">
         <v>97</v>
       </c>
-      <c r="D18" s="24"/>
-      <c r="E18" s="24"/>
-      <c r="F18" s="24"/>
-      <c r="G18" s="15"/>
-      <c r="H18" s="16" t="s">
+      <c r="D18" s="21"/>
+      <c r="E18" s="21"/>
+      <c r="F18" s="21"/>
+      <c r="G18" s="12"/>
+      <c r="H18" s="13" t="s">
         <v>98</v>
       </c>
-      <c r="I18" s="16"/>
-      <c r="J18" s="16" t="s">
+      <c r="I18" s="13"/>
+      <c r="J18" s="13" t="s">
         <v>64</v>
       </c>
-      <c r="K18" s="16" t="s">
+      <c r="K18" s="13" t="s">
         <v>82</v>
       </c>
-      <c r="L18" s="16" t="s">
+      <c r="L18" s="13" t="s">
         <v>99</v>
       </c>
-      <c r="M18" s="16" t="s">
+      <c r="M18" s="13" t="s">
         <v>100</v>
       </c>
-      <c r="N18" s="16"/>
-      <c r="O18" s="17" t="s">
+      <c r="N18" s="13"/>
+      <c r="O18" s="14" t="s">
         <v>85</v>
       </c>
-      <c r="P18" s="16" t="s">
+      <c r="P18" s="13" t="s">
         <v>101</v>
       </c>
-      <c r="Q18" s="12"/>
-    </row>
-    <row r="19" spans="2:17" ht="27.6" x14ac:dyDescent="0.3">
-      <c r="B19" s="13"/>
-      <c r="C19" s="24" t="s">
+      <c r="Q18" s="9"/>
+    </row>
+    <row r="19" spans="2:17" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="B19" s="10"/>
+      <c r="C19" s="21" t="s">
         <v>102</v>
       </c>
-      <c r="D19" s="24"/>
-      <c r="E19" s="24"/>
-      <c r="F19" s="24"/>
-      <c r="G19" s="15"/>
-      <c r="H19" s="16" t="s">
+      <c r="D19" s="21"/>
+      <c r="E19" s="21"/>
+      <c r="F19" s="21"/>
+      <c r="G19" s="12"/>
+      <c r="H19" s="13" t="s">
         <v>103</v>
       </c>
-      <c r="I19" s="16" t="s">
+      <c r="I19" s="13" t="s">
         <v>71</v>
       </c>
-      <c r="J19" s="16" t="s">
+      <c r="J19" s="13" t="s">
         <v>30</v>
       </c>
-      <c r="K19" s="16" t="s">
+      <c r="K19" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="L19" s="16" t="s">
+      <c r="L19" s="13" t="s">
         <v>104</v>
       </c>
-      <c r="M19" s="16" t="s">
+      <c r="M19" s="13" t="s">
         <v>105</v>
       </c>
-      <c r="N19" s="16" t="s">
+      <c r="N19" s="13" t="s">
         <v>106</v>
       </c>
-      <c r="O19" s="16"/>
-      <c r="P19" s="16" t="s">
+      <c r="O19" s="13"/>
+      <c r="P19" s="13" t="s">
         <v>107</v>
       </c>
-      <c r="Q19" s="12"/>
+      <c r="Q19" s="9"/>
     </row>
   </sheetData>
   <mergeCells count="9">
@@ -1647,76 +1647,76 @@
       <selection activeCell="C17" activeCellId="1" sqref="P18 C17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="2" width="8.5546875" customWidth="1"/>
-    <col min="3" max="3" width="41.21875" customWidth="1"/>
+    <col min="1" max="2" width="8.5703125" customWidth="1"/>
+    <col min="3" max="3" width="41.28515625" customWidth="1"/>
     <col min="4" max="4" width="28" customWidth="1"/>
     <col min="5" max="5" width="32" customWidth="1"/>
-    <col min="6" max="6" width="24.88671875" customWidth="1"/>
-    <col min="7" max="7" width="27.109375" customWidth="1"/>
-    <col min="8" max="1025" width="8.5546875" customWidth="1"/>
+    <col min="6" max="6" width="24.85546875" customWidth="1"/>
+    <col min="7" max="7" width="27.140625" customWidth="1"/>
+    <col min="8" max="1025" width="8.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="3:5" ht="38.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C3" s="1" t="s">
+    <row r="3" spans="3:5" ht="38.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C3" s="25" t="s">
         <v>24</v>
       </c>
-      <c r="D3" s="1"/>
-      <c r="E3" s="7" t="s">
+      <c r="D3" s="25"/>
+      <c r="E3" s="4" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="4" spans="3:5" x14ac:dyDescent="0.3">
-      <c r="C4" s="25" t="s">
+    <row r="4" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C4" s="22" t="s">
         <v>109</v>
       </c>
-      <c r="D4" s="25" t="s">
+      <c r="D4" s="22" t="s">
         <v>110</v>
       </c>
-      <c r="E4" s="25" t="s">
+      <c r="E4" s="22" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="5" spans="3:5" x14ac:dyDescent="0.3">
-      <c r="C5" s="16" t="s">
+    <row r="5" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C5" s="13" t="s">
         <v>112</v>
       </c>
-      <c r="D5" s="16" t="s">
+      <c r="D5" s="13" t="s">
         <v>113</v>
       </c>
-      <c r="E5" s="16" t="s">
+      <c r="E5" s="13" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="8" spans="3:5" ht="38.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C8" s="1" t="s">
+    <row r="8" spans="3:5" ht="38.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C8" s="25" t="s">
         <v>27</v>
       </c>
-      <c r="D8" s="1"/>
-      <c r="E8" s="7" t="s">
+      <c r="D8" s="25"/>
+      <c r="E8" s="4" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="9" spans="3:5" x14ac:dyDescent="0.3">
-      <c r="C9" s="25" t="s">
+    <row r="9" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C9" s="22" t="s">
         <v>109</v>
       </c>
-      <c r="D9" s="25" t="s">
+      <c r="D9" s="22" t="s">
         <v>110</v>
       </c>
-      <c r="E9" s="25" t="s">
+      <c r="E9" s="22" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="10" spans="3:5" x14ac:dyDescent="0.3">
-      <c r="C10" s="16" t="s">
+    <row r="10" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C10" s="13" t="s">
         <v>116</v>
       </c>
-      <c r="D10" s="16" t="s">
+      <c r="D10" s="13" t="s">
         <v>117</v>
       </c>
-      <c r="E10" s="16" t="s">
+      <c r="E10" s="13" t="s">
         <v>118</v>
       </c>
     </row>

</xml_diff>